<commit_message>
switching to production database
</commit_message>
<xml_diff>
--- a/Outputs/Course_Catalog_Review.xlsx
+++ b/Outputs/Course_Catalog_Review.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiasatterfield/Dev/Scholacity_Parser/Scholacity_Parser/Outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiasatterfield/Dev/Scholacity_Parser/Scholacity_Parser/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF30A09-41CA-ED45-BB85-6B7901448C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8C3839-64F1-CA4F-A046-CBF8CEA3569A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4480" yWindow="6620" windowWidth="39760" windowHeight="18940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3931,7 +3931,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:5" ht="32">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="32">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="32">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="32">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="32">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
+    <row r="10" spans="1:5" ht="32">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16">
+    <row r="16" spans="1:5" ht="32">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16">
+    <row r="19" spans="1:4" ht="32">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16">
+    <row r="22" spans="1:4" ht="32">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16">
+    <row r="24" spans="1:4" ht="32">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16">
+    <row r="25" spans="1:4" ht="32">
       <c r="A25" t="s">
         <v>87</v>
       </c>

</xml_diff>